<commit_message>
feat: update printing to console
</commit_message>
<xml_diff>
--- a/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
+++ b/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F3590F1-1D95-46C9-A047-36E622E1B9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64F01C89-7546-4F03-A88E-E2E49CFF275F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,45 @@
     <t>e9c101d0-f344-11ee-95ad-619443a476e1</t>
   </si>
   <si>
+    <t>CyberSec.Booster: Detection of a rogue DHCP server</t>
+  </si>
+  <si>
+    <t>T1557.003</t>
+  </si>
+  <si>
+    <t>SW_DAI-4</t>
+  </si>
+  <si>
+    <t>cbfe07a0-f345-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Password Guessing</t>
+  </si>
+  <si>
+    <t>T1110.001</t>
+  </si>
+  <si>
+    <t>SSH-5 SEC_LOGIN-4</t>
+  </si>
+  <si>
+    <t>d36fef60-f347-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Manipulation of the STP protocol</t>
+  </si>
+  <si>
+    <t>T1498.001</t>
+  </si>
+  <si>
+    <t>SPANTREE</t>
+  </si>
+  <si>
+    <t>267c1370-f346-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
     <t>CyberSec.Booster: MAC Flooding</t>
   </si>
   <si>
-    <t>T1498.001</t>
-  </si>
-  <si>
     <t>MACNOTIFY-6 PORT_SECURITY-2</t>
   </si>
   <si>
@@ -87,18 +120,6 @@
     <t>d884bc00-f343-11ee-95ad-619443a476e1</t>
   </si>
   <si>
-    <t>CyberSec.Booster: Password Guessing</t>
-  </si>
-  <si>
-    <t>T1110.001</t>
-  </si>
-  <si>
-    <t>SSH-5 SEC_LOGIN-4</t>
-  </si>
-  <si>
-    <t>d36fef60-f347-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
     <t>CyberSec.Booster: DNS data exfiltration</t>
   </si>
   <si>
@@ -108,18 +129,6 @@
     <t>8adc2400-f345-11ee-95ad-619443a476e1</t>
   </si>
   <si>
-    <t>CyberSec.Booster: Detection of a rogue DHCP server</t>
-  </si>
-  <si>
-    <t>T1557.003</t>
-  </si>
-  <si>
-    <t>SW_DAI-4</t>
-  </si>
-  <si>
-    <t>cbfe07a0-f345-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
     <t>CyberSec.Booster: Telnet Port Activity</t>
   </si>
   <si>
@@ -139,15 +148,6 @@
   </si>
   <si>
     <t>0007b730-f346-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Manipulation of the STP protocol</t>
-  </si>
-  <si>
-    <t>SPANTREE</t>
-  </si>
-  <si>
-    <t>267c1370-f346-11ee-95ad-619443a476e1</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A10" sqref="A10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,54 +587,57 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
@@ -648,7 +651,7 @@
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -659,19 +662,16 @@
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
feat: generate state to csv and fix parsing errors
</commit_message>
<xml_diff>
--- a/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
+++ b/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64F01C89-7546-4F03-A88E-E2E49CFF275F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA5DE15F-24A2-48A4-8898-E29B7A13930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,6 +57,30 @@
     <t>e9c101d0-f344-11ee-95ad-619443a476e1</t>
   </si>
   <si>
+    <t>CyberSec.Booster: Password Guessing</t>
+  </si>
+  <si>
+    <t>T1110.001</t>
+  </si>
+  <si>
+    <t>SSH-5 SEC_LOGIN-4</t>
+  </si>
+  <si>
+    <t>d36fef60-f347-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Manipulation of the STP protocol</t>
+  </si>
+  <si>
+    <t>T1498.001</t>
+  </si>
+  <si>
+    <t>SPANTREE</t>
+  </si>
+  <si>
+    <t>267c1370-f346-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
     <t>CyberSec.Booster: Detection of a rogue DHCP server</t>
   </si>
   <si>
@@ -69,28 +93,52 @@
     <t>cbfe07a0-f345-11ee-95ad-619443a476e1</t>
   </si>
   <si>
-    <t>CyberSec.Booster: Password Guessing</t>
-  </si>
-  <si>
-    <t>T1110.001</t>
-  </si>
-  <si>
-    <t>SSH-5 SEC_LOGIN-4</t>
-  </si>
-  <si>
-    <t>d36fef60-f347-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Manipulation of the STP protocol</t>
-  </si>
-  <si>
-    <t>T1498.001</t>
-  </si>
-  <si>
-    <t>SPANTREE</t>
-  </si>
-  <si>
-    <t>267c1370-f346-11ee-95ad-619443a476e1</t>
+    <t>CyberSec.Booster: Scanning ip blocks</t>
+  </si>
+  <si>
+    <t>T1595.001</t>
+  </si>
+  <si>
+    <t>eb158cb0-e54b-11ee-aad9-f582020d7fab</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Vulnerability Scanning</t>
+  </si>
+  <si>
+    <t>T1595.002</t>
+  </si>
+  <si>
+    <t>d884bc00-f343-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: DNS data exfiltration</t>
+  </si>
+  <si>
+    <t>T1071.004</t>
+  </si>
+  <si>
+    <t>8adc2400-f345-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Telnet Port Activity</t>
+  </si>
+  <si>
+    <t>TA0011</t>
+  </si>
+  <si>
+    <t>9610b910-f347-11ee-95ad-619443a476e1</t>
+  </si>
+  <si>
+    <t>CyberSec.Booster: Manipulation of the DTP protocol</t>
+  </si>
+  <si>
+    <t>T1557</t>
+  </si>
+  <si>
+    <t>DTP-5</t>
+  </si>
+  <si>
+    <t>0007b730-f346-11ee-95ad-619443a476e1</t>
   </si>
   <si>
     <t>CyberSec.Booster: MAC Flooding</t>
@@ -100,54 +148,6 @@
   </si>
   <si>
     <t>0aab2540-f347-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Scanning ip blocks</t>
-  </si>
-  <si>
-    <t>T1595.001</t>
-  </si>
-  <si>
-    <t>eb158cb0-e54b-11ee-aad9-f582020d7fab</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Vulnerability Scanning</t>
-  </si>
-  <si>
-    <t>T1595.002</t>
-  </si>
-  <si>
-    <t>d884bc00-f343-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: DNS data exfiltration</t>
-  </si>
-  <si>
-    <t>T1071.004</t>
-  </si>
-  <si>
-    <t>8adc2400-f345-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Telnet Port Activity</t>
-  </si>
-  <si>
-    <t>TA0011</t>
-  </si>
-  <si>
-    <t>9610b910-f347-11ee-95ad-619443a476e1</t>
-  </si>
-  <si>
-    <t>CyberSec.Booster: Manipulation of the DTP protocol</t>
-  </si>
-  <si>
-    <t>T1557</t>
-  </si>
-  <si>
-    <t>SWITCHPORT-5</t>
-  </si>
-  <si>
-    <t>0007b730-f346-11ee-95ad-619443a476e1</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -613,9 +613,6 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
@@ -640,7 +637,7 @@
       <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -651,7 +648,7 @@
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -662,16 +659,19 @@
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
feat: fix errors in config file and generate state
</commit_message>
<xml_diff>
--- a/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
+++ b/Bc.CyberSec.Detection.Booster.CLI/Init/UseCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA5DE15F-24A2-48A4-8898-E29B7A13930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98CE2408-2401-4C43-B507-5F8D335FED88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>T1557.002</t>
   </si>
   <si>
-    <t>SW_MATM-4 SW_DAI-4</t>
+    <t>SW_MATM SW_DAI</t>
   </si>
   <si>
     <t>e9c101d0-f344-11ee-95ad-619443a476e1</t>
@@ -63,7 +63,7 @@
     <t>T1110.001</t>
   </si>
   <si>
-    <t>SSH-5 SEC_LOGIN-4</t>
+    <t>SSH SEC_LOGIN</t>
   </si>
   <si>
     <t>d36fef60-f347-11ee-95ad-619443a476e1</t>
@@ -87,7 +87,7 @@
     <t>T1557.003</t>
   </si>
   <si>
-    <t>SW_DAI-4</t>
+    <t>SW_DAI</t>
   </si>
   <si>
     <t>cbfe07a0-f345-11ee-95ad-619443a476e1</t>
@@ -135,7 +135,7 @@
     <t>T1557</t>
   </si>
   <si>
-    <t>DTP-5</t>
+    <t>DTP</t>
   </si>
   <si>
     <t>0007b730-f346-11ee-95ad-619443a476e1</t>
@@ -144,7 +144,7 @@
     <t>CyberSec.Booster: MAC Flooding</t>
   </si>
   <si>
-    <t>MACNOTIFY-6 PORT_SECURITY-2</t>
+    <t>MACNOTIFY PORT_SECURITY</t>
   </si>
   <si>
     <t>0aab2540-f347-11ee-95ad-619443a476e1</t>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>